<commit_message>
Se invocan stored procedures desde el controlador  de C#
</commit_message>
<xml_diff>
--- a/Documentación/Cronograma SistemaMixioteO.xlsx
+++ b/Documentación/Cronograma SistemaMixioteO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3 Bibliotecas\Desktop\Proyeco Mixiote\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELFINO\Google Drive\Proyecto Mixiote\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C7207AB8-B059-4F93-8C02-F9CC8E26BEE4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A9018E7A-01B8-4B7C-9DC7-A383390A94A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6750" activeTab="1" xr2:uid="{F0F7A659-F9ED-4026-AC19-587005F2BF54}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>domingo</t>
   </si>
@@ -1115,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F683C4-A1DB-4881-BC69-209457536E11}">
-  <dimension ref="B2:H16"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,8 +1148,8 @@
         <v>14</v>
       </c>
       <c r="H3" s="11">
-        <f>COUNT(C4:C16)</f>
-        <v>11</v>
+        <f>COUNT(C4:C22)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -1166,8 +1166,8 @@
         <v>13</v>
       </c>
       <c r="H4" s="13">
-        <f>SUM(D4:D16)</f>
-        <v>35.5</v>
+        <f>SUM(D4:D22)</f>
+        <v>50.5</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="H7" s="17">
         <f>H4*H6</f>
-        <v>3328.125</v>
+        <v>4734.375</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -1298,6 +1298,50 @@
       </c>
       <c r="D16" s="20">
         <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="19">
+        <v>4</v>
+      </c>
+      <c r="D17" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="19">
+        <v>7</v>
+      </c>
+      <c r="D19" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="19">
+        <v>8</v>
+      </c>
+      <c r="D20" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="19">
+        <v>11</v>
+      </c>
+      <c r="D22" s="20">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se optimizó el método crearMesas del formulario InicializarMesas
</commit_message>
<xml_diff>
--- a/Documentación/Cronograma SistemaMixioteO.xlsx
+++ b/Documentación/Cronograma SistemaMixioteO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELFINO\Google Drive\Proyecto Mixiote\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A9018E7A-01B8-4B7C-9DC7-A383390A94A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7C3BF427-4CBD-4CE7-B1B6-8C6B2FFB7202}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6750" activeTab="1" xr2:uid="{F0F7A659-F9ED-4026-AC19-587005F2BF54}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>domingo</t>
   </si>
@@ -1115,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F683C4-A1DB-4881-BC69-209457536E11}">
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,8 +1148,8 @@
         <v>14</v>
       </c>
       <c r="H3" s="11">
-        <f>COUNT(C4:C22)</f>
-        <v>15</v>
+        <f>COUNT(C4:C26)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -1166,8 +1166,8 @@
         <v>13</v>
       </c>
       <c r="H4" s="13">
-        <f>SUM(D4:D22)</f>
-        <v>50.5</v>
+        <f>SUM(D4:D26)</f>
+        <v>64.5</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="H7" s="17">
         <f>H4*H6</f>
-        <v>4734.375</v>
+        <v>6046.875</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -1342,6 +1342,39 @@
       </c>
       <c r="D22" s="20">
         <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="19">
+        <v>12</v>
+      </c>
+      <c r="D23" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="19">
+        <v>14</v>
+      </c>
+      <c r="D25" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="19">
+        <v>15</v>
+      </c>
+      <c r="D26" s="20">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Śe amplió el diseño CreacionDeCuenta. Se agregaron las opciones; hora de llegada, tiempo transcurrido
</commit_message>
<xml_diff>
--- a/Documentación/Cronograma SistemaMixioteO.xlsx
+++ b/Documentación/Cronograma SistemaMixioteO.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELFINO\Google Drive\Proyecto Mixiote\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7C3BF427-4CBD-4CE7-B1B6-8C6B2FFB7202}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B83762-02DF-4BC6-B2AC-026970B0F67A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6750" activeTab="1" xr2:uid="{F0F7A659-F9ED-4026-AC19-587005F2BF54}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6750" activeTab="2" xr2:uid="{F0F7A659-F9ED-4026-AC19-587005F2BF54}"/>
   </bookViews>
   <sheets>
     <sheet name="Diciembre2018" sheetId="1" r:id="rId1"/>
-    <sheet name="Horas2018" sheetId="2" r:id="rId2"/>
+    <sheet name="Enero2019" sheetId="3" r:id="rId2"/>
+    <sheet name="Horas2018" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,8 +26,137 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>DELFINO</author>
+  </authors>
+  <commentList>
+    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{F550E679-94B0-4439-BC58-43A3C9FA8C1E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DELFINO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">INV. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Herencia y Polimorfismo
+Se buscaron ejemplos de ambos para el entorno de Java y .Net.
+Los ejemplos realizados se encuentran guardados en "mis Documentos/1. PROGRAMACIÓN"
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{0C962CA7-CED9-46AD-93CE-75FD0E603948}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DELFINO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">C.U: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CreacionDeCuenta
+Se trabajó con la recuperación de datos de la cuenta, una vez que el usuario hace clic en una de las mesas ocupadas del C.U InicializacionDeMesas.
+Se cambió el tipo de dato a las fechas y horas de la tabla "Folio"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="0" shapeId="0" xr:uid="{80410444-920C-49D0-A192-84EA6E395805}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>DELFINO
+C.U:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> CreacionDeCuenta
+Selección de los combos (mesa y mesero) y asignación dentro de las cajas de texto.
+Se borró el avance del diseño.
+Se creó la rama "Diseño" en el repositorio de GitHub.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
   <si>
     <t>domingo</t>
   </si>
@@ -81,12 +211,15 @@
   <si>
     <t>Enero</t>
   </si>
+  <si>
+    <t>Días de un mes distinto al trabajado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +258,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,8 +324,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -271,11 +438,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,11 +519,290 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -592,28 +1067,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5319A39-BB33-445F-91C7-D6D495EE86FC}" name="Tabla1" displayName="Tabla1" ref="B3:H9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5319A39-BB33-445F-91C7-D6D495EE86FC}" name="Tabla1" displayName="Tabla1" ref="B3:H9" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="B3:H9" xr:uid="{9ED27164-FC51-4761-810C-1B34356AEB7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B2CF6E80-84A7-49D8-9D98-F7E4328A977D}" name="domingo" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{E1D8FCD4-D404-4206-8010-10428AF5F87F}" name="lunes" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{E0776291-4918-4018-8333-B376D0BB0E06}" name="martes" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{D81D8E05-9327-42AC-9CD0-B671B549BA5F}" name="miércoles" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{6306D711-307C-4085-8DAB-5ADC3616DFB0}" name="jueves" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{1DFAEC14-3F0D-4C93-8842-9EE46DB51FAE}" name="viernes" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{EACF9D27-C6B8-4D55-A7EB-134F25EEB4DD}" name="sábado" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{B2CF6E80-84A7-49D8-9D98-F7E4328A977D}" name="domingo" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{E1D8FCD4-D404-4206-8010-10428AF5F87F}" name="lunes" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{E0776291-4918-4018-8333-B376D0BB0E06}" name="martes" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{D81D8E05-9327-42AC-9CD0-B671B549BA5F}" name="miércoles" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{6306D711-307C-4085-8DAB-5ADC3616DFB0}" name="jueves" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{1DFAEC14-3F0D-4C93-8842-9EE46DB51FAE}" name="viernes" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{EACF9D27-C6B8-4D55-A7EB-134F25EEB4DD}" name="sábado" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CA13C63B-6EB6-40CC-83C1-CD8C2C0ACE7F}" name="Tabla2" displayName="Tabla2" ref="B3:D12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58A62DFA-8D0B-4AFF-A691-24DEE466C0C9}" name="Tabla3" displayName="Tabla3" ref="B3:H8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="9">
+  <autoFilter ref="B3:H8" xr:uid="{58C88DCE-DF04-430A-B36E-DFC7D8F377DD}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{47C515D5-DCD3-496A-9BB4-937E9B12AF4D}" name="domingo" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{57D43009-5F96-4D65-AAB2-837D24936A12}" name="lunes" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{25833DB1-5C7D-400E-9029-51C37DBBD06A}" name="martes" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{5F1544F6-D3A3-4ACA-807D-C90555847BC2}" name="miércoles" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{E2FCDF60-85E2-48A4-BAE5-F4514B9A0E51}" name="jueves" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{A03D3C0A-BA96-4471-99C4-DD04D97288AB}" name="viernes" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{7A532242-1700-4151-AF1A-1E2ACA065E2E}" name="sábado" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CA13C63B-6EB6-40CC-83C1-CD8C2C0ACE7F}" name="Tabla2" displayName="Tabla2" ref="B3:D12" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="B3:D12" xr:uid="{A45A35C4-7B7F-4341-98D8-563885D85FF2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{615DF9C7-B6F5-400B-BA39-734C0FE76DD7}" name="Mes" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{087BC10B-2AFF-4259-893F-4D76B5EF757A}" name="Día " dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{9B1C9D77-643E-46B3-BC33-D92832687BD2}" name="Horas" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{615DF9C7-B6F5-400B-BA39-734C0FE76DD7}" name="Mes" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{087BC10B-2AFF-4259-893F-4D76B5EF757A}" name="Día " dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{9B1C9D77-643E-46B3-BC33-D92832687BD2}" name="Horas" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -916,10 +1407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0181A26C-BE0A-42D6-BF77-8696F1A888EE}">
-  <dimension ref="B3:H16"/>
+  <dimension ref="B3:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,18 +1554,18 @@
       <c r="F8" s="3">
         <v>27</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3">
         <v>28</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="3">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>30</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>31</v>
       </c>
       <c r="D9" s="2">
@@ -1102,6 +1593,12 @@
       <c r="B16" s="5"/>
       <c r="C16" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="28"/>
+      <c r="C17" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1114,11 +1611,193 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F683C4-A1DB-4881-BC69-209457536E11}">
-  <dimension ref="B2:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AD9E93-F930-4CB2-838A-29A503B6AE96}">
+  <dimension ref="B3:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="23">
+        <v>30</v>
+      </c>
+      <c r="C4" s="23">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>4</v>
+      </c>
+      <c r="H4" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="25">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8</v>
+      </c>
+      <c r="E5" s="25">
+        <v>9</v>
+      </c>
+      <c r="F5" s="24">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="25">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3">
+        <v>15</v>
+      </c>
+      <c r="E6" s="25">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3">
+        <v>18</v>
+      </c>
+      <c r="H6" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="25">
+        <v>20</v>
+      </c>
+      <c r="C7" s="25">
+        <v>21</v>
+      </c>
+      <c r="D7" s="24">
+        <v>22</v>
+      </c>
+      <c r="E7" s="25">
+        <v>23</v>
+      </c>
+      <c r="F7" s="24">
+        <v>24</v>
+      </c>
+      <c r="G7" s="25">
+        <v>25</v>
+      </c>
+      <c r="H7" s="24">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="25">
+        <v>27</v>
+      </c>
+      <c r="C8" s="25">
+        <v>28</v>
+      </c>
+      <c r="D8" s="24">
+        <v>29</v>
+      </c>
+      <c r="E8" s="25">
+        <v>30</v>
+      </c>
+      <c r="F8" s="24">
+        <v>31</v>
+      </c>
+      <c r="G8" s="23">
+        <v>1</v>
+      </c>
+      <c r="H8" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="28"/>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F683C4-A1DB-4881-BC69-209457536E11}">
+  <dimension ref="B2:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,8 +1827,8 @@
         <v>14</v>
       </c>
       <c r="H3" s="11">
-        <f>COUNT(C4:C26)</f>
-        <v>18</v>
+        <f>COUNT(C4:C30)</f>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -1166,8 +1845,8 @@
         <v>13</v>
       </c>
       <c r="H4" s="13">
-        <f>SUM(D4:D26)</f>
-        <v>64.5</v>
+        <f>SUM(D4:D30)</f>
+        <v>76.5</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -1209,7 +1888,7 @@
       </c>
       <c r="H7" s="17">
         <f>H4*H6</f>
-        <v>6046.875</v>
+        <v>7171.875</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -1377,11 +2056,45 @@
         <v>6</v>
       </c>
     </row>
+    <row r="28" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="19">
+        <v>17</v>
+      </c>
+      <c r="D28" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="19">
+        <v>18</v>
+      </c>
+      <c r="D29" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="19">
+        <v>19</v>
+      </c>
+      <c r="D30" s="20">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>